<commit_message>
correcoes parte da gest func
</commit_message>
<xml_diff>
--- a/Use Cases - Gestão de Funcionários.xlsx
+++ b/Use Cases - Gestão de Funcionários.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\MIEI\3º Ano\1º Semestre\Desenvolvimento de Sistemas de Software\Projeto\dss-projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedroferreira/Desktop/DSS/dss-projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F86D051-CA7A-444B-9C90-4C7564D658B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Registar Funcionário" sheetId="20" r:id="rId1"/>
     <sheet name="Remover Funcionário" sheetId="21" r:id="rId2"/>
     <sheet name="Alterar Funcionário" sheetId="22" r:id="rId3"/>
+    <sheet name="Identificar Funcionário" sheetId="26" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>Actor input</t>
   </si>
@@ -69,23 +69,10 @@
     <t>Funcionário registado</t>
   </si>
   <si>
-    <t>2. Verifica se o funcionário já existe</t>
-  </si>
-  <si>
-    <t>3. Pede para inserir os dados 
-sobre o mesmo</t>
-  </si>
-  <si>
-    <t>5. Regista o funcionário</t>
-  </si>
-  <si>
     <t>Remover Funcionário</t>
   </si>
   <si>
     <t>Funcionário Removido</t>
-  </si>
-  <si>
-    <t>1. Indica o funcionário a remover</t>
   </si>
   <si>
     <t>2. Verifica se está inserido no 
@@ -118,63 +105,7 @@
     <t>5. Atualiza funcionário</t>
   </si>
   <si>
-    <t>3.1. Não confirma os dados</t>
-  </si>
-  <si>
-    <t>2. Verifica se está inserido no sistema</t>
-  </si>
-  <si>
-    <t>3. Apresenta a informação do funcionário</t>
-  </si>
-  <si>
-    <t>3.2. Informa que a remoção foi cancelada</t>
-  </si>
-  <si>
     <t>2.1. Informa que o funcionário não está registado e cancela o processo</t>
-  </si>
-  <si>
-    <t>Cenário 
-Excepção 1 
-[funcionário não registado] 
-(passo 2)</t>
-  </si>
-  <si>
-    <t>Cenário 
-Excepção 2 
-[não confirma] 
-(passo 3)</t>
-  </si>
-  <si>
-    <t>1. Indica ID do novo funcionário</t>
-  </si>
-  <si>
-    <t>4. Insere a informação necessária</t>
-  </si>
-  <si>
-    <t>2.1. Informa que o funcionário
-já se encontra inserido</t>
-  </si>
-  <si>
-    <t>2.2. Cancela registo</t>
-  </si>
-  <si>
-    <t>4.1. Não preenche os campos
- todos</t>
-  </si>
-  <si>
-    <t>4.3. Cancela registo</t>
-  </si>
-  <si>
-    <t>Cenário 
-Excepção 2
- [campos por preencher] 
-(passo 4)</t>
-  </si>
-  <si>
-    <t>Cenário 
-Excepção 1 
-[funcionário já inserido] 
-(passo 2)</t>
   </si>
   <si>
     <t>Cenário 
@@ -192,18 +123,76 @@
     <t>4.1. Indica que não quer fazer alterações</t>
   </si>
   <si>
-    <t xml:space="preserve">4.2. Informa que falta preencher
-informação </t>
-  </si>
-  <si>
     <t>4.2. Informa que o funcionário
  permaneceu inalterado</t>
+  </si>
+  <si>
+    <t>1. Indica dados do funcionário</t>
+  </si>
+  <si>
+    <t>2. Regista Funcionário</t>
+  </si>
+  <si>
+    <t>3. Informa que funcionário foi inserido com sucesso</t>
+  </si>
+  <si>
+    <t>Cenário 
+Excepção 1 
+[dados por preencher] 
+(passo 2)</t>
+  </si>
+  <si>
+    <t>2.1. Informa que faltam preencher dados</t>
+  </si>
+  <si>
+    <t>1. &lt;&lt; include &gt;&gt; Identificar Funcionário</t>
+  </si>
+  <si>
+    <t>2. Indica que quer remover 
+funcionário</t>
+  </si>
+  <si>
+    <t>3. Pede para confirmar a remoção</t>
+  </si>
+  <si>
+    <t>6. Indica que funcionário foi removido
+ com sucesso</t>
+  </si>
+  <si>
+    <t>Cenário 
+Excepção 1 
+[não confirma] 
+(passo 4)</t>
+  </si>
+  <si>
+    <t>4.1. Cancela remoção</t>
+  </si>
+  <si>
+    <t>4.2. Informa que a remoção foi cancelada</t>
+  </si>
+  <si>
+    <t>Identificar Funcionário</t>
+  </si>
+  <si>
+    <t>Funcionário identificado</t>
+  </si>
+  <si>
+    <t>1. Obtém lista de funcionários</t>
+  </si>
+  <si>
+    <t>2. Apresenta lista de funcionários</t>
+  </si>
+  <si>
+    <t>3. Escolhe funcionário a consultar</t>
+  </si>
+  <si>
+    <t>4. Apresenta dados do funcionário</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -269,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -427,6 +416,19 @@
     </border>
     <border>
       <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="medium">
@@ -446,7 +448,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -484,6 +486,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -508,14 +518,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
@@ -833,59 +842,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="4" width="34.875" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="26"/>
+    </row>
+    <row r="6" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="26"/>
+    </row>
+    <row r="7" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="23" t="s">
+      <c r="D7" s="26"/>
+    </row>
+    <row r="8" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -895,110 +904,70 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="24"/>
-      <c r="C9" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="29"/>
+    <row r="9" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="28"/>
+      <c r="C9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="21"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="24"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="24"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="24"/>
-      <c r="C12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="28"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="28"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="24"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="24"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="20"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="20"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="14"/>
-    </row>
-    <row r="19" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="19"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="20"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="24"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
+  <mergeCells count="6">
+    <mergeCell ref="B12:B15"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B8:B14"/>
+    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1006,59 +975,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B4:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.625" customWidth="1"/>
-    <col min="3" max="3" width="33.625" customWidth="1"/>
-    <col min="4" max="4" width="39.375" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="26"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="26"/>
+    </row>
+    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="26"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="22"/>
-    </row>
-    <row r="9" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="23" t="s">
+      <c r="C8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="26"/>
+    </row>
+    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -1068,80 +1037,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="24"/>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
+    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="28"/>
+      <c r="C10" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="24"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="24"/>
+    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="28"/>
+      <c r="C11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="28"/>
       <c r="C12" s="5"/>
       <c r="D12" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="24"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="28"/>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="24"/>
+    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="28"/>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="24"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="28"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:6" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="20"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="20"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
+      <c r="D15" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="14"/>
+    </row>
+    <row r="17" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="23"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="24"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
@@ -1154,59 +1115,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="33.625" customWidth="1"/>
-    <col min="4" max="4" width="35.125" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="22"/>
+      <c r="C4" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="26"/>
+    </row>
+    <row r="6" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="26"/>
+    </row>
+    <row r="7" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="23" t="s">
+      <c r="C7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="26"/>
+    </row>
+    <row r="8" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -1216,70 +1177,70 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="24"/>
+    <row r="9" spans="2:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="28"/>
       <c r="C9" s="11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="24"/>
+    <row r="10" spans="2:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="28"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="24"/>
+      <c r="D10" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="28"/>
       <c r="C11" s="5"/>
       <c r="D11" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="24"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="28"/>
       <c r="C12" s="11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="24"/>
+    <row r="13" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="28"/>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="24"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="28"/>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="2:6" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="2:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="25" t="s">
-        <v>41</v>
+    <row r="16" spans="2:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>23</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:4" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="26"/>
+    <row r="17" spans="2:4" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="30"/>
       <c r="C17" s="6"/>
       <c r="D17" s="13" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1294,4 +1255,119 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="26"/>
+    </row>
+    <row r="5" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="26"/>
+    </row>
+    <row r="6" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="26"/>
+    </row>
+    <row r="7" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="26"/>
+    </row>
+    <row r="8" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="28"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="28"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="28"/>
+      <c r="C11" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="28"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B8:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>